<commit_message>
Ⅰ. ExcelController.java excelToFileName method update Ⅱ. ExcelReadDTO.java new add Ⅲ. excelToFileName.html file list upload add
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/ExcelTemplate.xlsx
+++ b/src/main/resources/static/excel/ExcelTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Company\Project\All_Utils\all_utils\src\main\resources\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD97E5-A496-4E07-971B-8A2A7AD14E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24289074-7C49-44DF-9871-D525A1F66AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A34C6457-BECC-4723-9AD7-4D0E309F6458}"/>
   </bookViews>
@@ -168,20 +168,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,25 +500,25 @@
   <dimension ref="B1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="1.625" customWidth="1"/>
-    <col min="2" max="2" width="17.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="9.9499999999999993" customHeight="1" thickBot="1">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:3" ht="18" thickTop="1" thickBot="1">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>